<commit_message>
added environmental control in new sheet
</commit_message>
<xml_diff>
--- a/testdata/data-UAT.xlsx
+++ b/testdata/data-UAT.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dolphin_Demo\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CAA8EC-A73F-4C3D-82F9-C64A83F79D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BDDE94-E25E-4DF1-A8E0-00775C4580D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15B07E59-FCAF-4B6B-B18A-7E99B4CB5809}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{15B07E59-FCAF-4B6B-B18A-7E99B4CB5809}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EnvControl" sheetId="2" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>email</t>
   </si>
@@ -86,9 +87,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>qa,uat</t>
-  </si>
-  <si>
     <t>qa</t>
   </si>
   <si>
@@ -99,6 +97,12 @@
   </si>
   <si>
     <t>test1111</t>
+  </si>
+  <si>
+    <t>execute</t>
+  </si>
+  <si>
+    <t>dev</t>
   </si>
 </sst>
 </file>
@@ -507,11 +511,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A62C67-37CE-4679-913B-3665A8AE10FD}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB67A657-7D89-4CCF-A23A-C58C823BF288}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +603,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -569,7 +620,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -586,7 +637,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -603,15 +654,15 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -620,7 +671,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>